<commit_message>
added new conditions and notes section at top
</commit_message>
<xml_diff>
--- a/resources/MBTA_TEMPLATE.xlsx
+++ b/resources/MBTA_TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\Programming\python\WOIDS\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB78CFE5-E4C8-405A-AACB-1B4A99231805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B9E48A-FE29-44BB-B4DF-25844AAA5CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="10155" windowWidth="16200" windowHeight="14100" xr2:uid="{6C08E104-9442-4E06-87D5-3C5A41D74CD0}"/>
+    <workbookView xWindow="-16200" yWindow="-3945" windowWidth="16200" windowHeight="14100" xr2:uid="{6C08E104-9442-4E06-87D5-3C5A41D74CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="22">
   <si>
     <t>RAIL LINE</t>
   </si>
@@ -77,9 +77,6 @@
     <t>SOLUTION TEXT</t>
   </si>
   <si>
-    <t>CONDITION STATE (1-4)</t>
-  </si>
-  <si>
     <t>PROBLEM TITLE</t>
   </si>
   <si>
@@ -99,13 +96,22 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>TUNNEL ID NUM (TIN)</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>CONDITION STATE (1-5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +162,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -189,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -217,6 +230,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +550,7 @@
     <tableColumn id="3" xr3:uid="{5D15C5EE-CA33-4963-853D-E90ED4A44306}" name="ID" dataDxfId="55"/>
     <tableColumn id="4" xr3:uid="{CA11D2E4-3A9C-4555-B4DE-64C636F6C791}" name="ROOM" dataDxfId="54"/>
     <tableColumn id="5" xr3:uid="{D9E0E1D4-4A97-4C5E-912F-D028472535C7}" name="EQUIPMENT ID" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{93212AF1-E91F-41EE-8331-5776F8932897}" name="CONDITION STATE (1-4)" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{93212AF1-E91F-41EE-8331-5776F8932897}" name="CONDITION STATE (1-5)" dataDxfId="52"/>
     <tableColumn id="7" xr3:uid="{83C073F3-6032-402D-9504-5535BB194AB9}" name="PROBLEM TITLE" dataDxfId="51"/>
     <tableColumn id="8" xr3:uid="{BAED3D3A-4E9F-4D52-B9AD-BF13F17C5185}" name="PROBLEM DESCRIPTION" dataDxfId="50"/>
     <tableColumn id="9" xr3:uid="{E6D85574-79A5-4E05-BDD5-456D38344E2E}" name="SOLUTION TITLE" dataDxfId="49"/>
@@ -553,7 +569,7 @@
     <tableColumn id="3" xr3:uid="{1ED2EC78-8DE3-40CE-B7ED-75080EBB1AFC}" name="ID" dataDxfId="43"/>
     <tableColumn id="4" xr3:uid="{B1922870-E1C9-4E18-A396-24B18C4E7749}" name="ROOM" dataDxfId="42"/>
     <tableColumn id="5" xr3:uid="{8035DFCE-BB95-4350-9B42-49A1D6AC4C0F}" name="EQUIPMENT ID" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{C12AC32B-B4AA-45B8-8C20-71810D668A3B}" name="CONDITION STATE (1-4)" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{C12AC32B-B4AA-45B8-8C20-71810D668A3B}" name="CONDITION STATE (1-5)" dataDxfId="40"/>
     <tableColumn id="7" xr3:uid="{331E44DF-6A28-418E-93BD-2DAE35A13D16}" name="PROBLEM TITLE" dataDxfId="39"/>
     <tableColumn id="8" xr3:uid="{7C4601A3-1EC1-472A-BA45-F32D20DD9272}" name="PROBLEM DESCRIPTION" dataDxfId="38"/>
     <tableColumn id="9" xr3:uid="{B0D6C0B1-ACA6-45E2-9EB5-0A568C22A588}" name="SOLUTION TITLE" dataDxfId="37"/>
@@ -572,7 +588,7 @@
     <tableColumn id="3" xr3:uid="{38F45304-B5C3-4F84-ABFE-69D007167950}" name="ID" dataDxfId="31"/>
     <tableColumn id="4" xr3:uid="{CD5812F5-04DE-44FC-8FA1-4F776CC815F9}" name="ROOM" dataDxfId="30"/>
     <tableColumn id="5" xr3:uid="{84D9B338-5DB1-4E00-9409-F4C94196884B}" name="EQUIPMENT ID" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{E408209D-964D-439B-ACD0-D2D41BDAFBC5}" name="CONDITION STATE (1-4)" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{E408209D-964D-439B-ACD0-D2D41BDAFBC5}" name="CONDITION STATE (1-5)" dataDxfId="28"/>
     <tableColumn id="7" xr3:uid="{C34146A8-A3EB-4FF9-8156-9502CDF8444C}" name="PROBLEM TITLE" dataDxfId="27"/>
     <tableColumn id="8" xr3:uid="{C24811CA-D0A9-42FC-9177-92A703CAE7EE}" name="PROBLEM DESCRIPTION" dataDxfId="26"/>
     <tableColumn id="9" xr3:uid="{DD1B58F3-572B-4808-B093-471EDAD9F182}" name="SOLUTION TITLE" dataDxfId="25"/>
@@ -591,7 +607,7 @@
     <tableColumn id="3" xr3:uid="{7B3CDFB5-12A9-4CBE-BD02-A17C0F2F0D71}" name="ID" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{CE032F65-79C2-4C81-A853-1B59EB1EAA63}" name="ROOM" dataDxfId="18"/>
     <tableColumn id="5" xr3:uid="{225A991A-6196-4AD2-AC1F-E325839B2843}" name="EQUIPMENT ID" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{9D05CD25-B8BA-41E5-B74D-F4B9D82E8CB2}" name="CONDITION STATE (1-4)" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{9D05CD25-B8BA-41E5-B74D-F4B9D82E8CB2}" name="CONDITION STATE (1-5)" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{F580E3FB-450A-4ADA-AC15-4AC961B89E34}" name="PROBLEM TITLE" dataDxfId="15"/>
     <tableColumn id="8" xr3:uid="{BF33B6AB-DF7A-47CE-8E3C-0939F63AF1F1}" name="PROBLEM DESCRIPTION" dataDxfId="14"/>
     <tableColumn id="9" xr3:uid="{1CBFD986-B4F3-46DE-9A4F-42EEFE7D0C2F}" name="SOLUTION TITLE" dataDxfId="13"/>
@@ -610,7 +626,7 @@
     <tableColumn id="3" xr3:uid="{A13C1FF4-9937-4558-B690-49C490131BE1}" name="ID" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{7972F4D0-36C0-47EA-AB14-D85BFED84973}" name="ROOM" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{B8EF4376-C6D4-4C52-B88C-83F8229A83F1}" name="EQUIPMENT ID" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{0FAD46BC-625B-4882-A850-C8FE88ACCEBD}" name="CONDITION STATE (1-4)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{0FAD46BC-625B-4882-A850-C8FE88ACCEBD}" name="CONDITION STATE (1-5)" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{1BCD0ACB-046F-4C09-86A9-C248A79D9595}" name="PROBLEM TITLE" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{83126D4C-D57B-4239-94AD-9921F322133E}" name="PROBLEM DESCRIPTION" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{7903F4A3-CA28-4F0F-BE67-303FACE33668}" name="SOLUTION TITLE" dataDxfId="1"/>
@@ -952,13 +968,17 @@
       <c r="B3" s="10"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+    <row r="4" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -968,6 +988,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -977,7 +998,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,13 +1032,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
@@ -1028,7 +1049,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1040,7 +1061,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1052,7 +1073,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -1064,7 +1085,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -1076,7 +1097,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -1100,7 +1121,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,13 +1155,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
@@ -1151,7 +1172,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1163,7 +1184,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1175,7 +1196,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -1187,7 +1208,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -1199,7 +1220,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -1223,7 +1244,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,13 +1278,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
@@ -1274,7 +1295,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1286,7 +1307,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1298,7 +1319,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -1310,7 +1331,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -1322,7 +1343,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -1346,7 +1367,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,13 +1401,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
@@ -1397,7 +1418,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1409,7 +1430,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1421,7 +1442,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -1433,7 +1454,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -1445,7 +1466,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -1469,7 +1490,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,13 +1524,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
@@ -1520,7 +1541,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1532,7 +1553,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1544,7 +1565,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -1556,7 +1577,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -1568,7 +1589,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>

</xml_diff>